<commit_message>
Database update (GHG, Water and Land)
</commit_message>
<xml_diff>
--- a/CIVICS_Ghana/IO_Ghana/Pumpfed Irrigation for Maize/Shock1_inputs.xlsx
+++ b/CIVICS_Ghana/IO_Ghana/Pumpfed Irrigation for Maize/Shock1_inputs.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gollinucci\Documents\GitHub\CIVICS\CIVICS_Ghana\IO_Ghana\Pumpfed Irrigation for Maize\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3DF248-54D5-438A-AD6C-8125D7333A35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F433D14-4D01-4F08-9A95-62C8A7FA191E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-5445" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-5445" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="indeces" sheetId="1" r:id="rId1"/>
     <sheet name="main" sheetId="2" r:id="rId2"/>
     <sheet name="Y" sheetId="3" r:id="rId3"/>
     <sheet name="VA" sheetId="4" r:id="rId4"/>
-    <sheet name="Z" sheetId="5" r:id="rId5"/>
+    <sheet name="S" sheetId="6" r:id="rId5"/>
+    <sheet name="Z" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="141">
   <si>
     <t>Maize</t>
   </si>
@@ -412,9 +413,6 @@
     <t>US Dollars / Ghanaian Cedi forex @2014</t>
   </si>
   <si>
-    <t>Deflation rate from 2020 to 2014</t>
-  </si>
-  <si>
     <t>https://www.in2013dollars.com/us/inflation/</t>
   </si>
   <si>
@@ -451,7 +449,16 @@
     <t>Absolute</t>
   </si>
   <si>
-    <t>calculation</t>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>conversion</t>
+  </si>
+  <si>
+    <t>Investment in wells @2012</t>
+  </si>
+  <si>
+    <t>Inflation rate from 2012 to 2015</t>
   </si>
 </sst>
 </file>
@@ -536,7 +543,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -560,6 +567,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1539,8 +1547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1550,9 +1558,8 @@
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
@@ -1632,10 +1639,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
+        <v>139</v>
       </c>
       <c r="C4" s="4">
         <v>449.5259858834267</v>
@@ -1652,7 +1659,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
         <v>124</v>
@@ -1669,19 +1676,19 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="C6">
-        <v>0.91</v>
+        <v>1.03</v>
       </c>
       <c r="D6" t="s">
         <v>112</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -1699,10 +1706,13 @@
         <v>115</v>
       </c>
       <c r="I7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J7" t="s">
         <v>138</v>
+      </c>
+      <c r="K7" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -1718,8 +1728,20 @@
       <c r="D8" t="s">
         <v>112</v>
       </c>
+      <c r="E8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="G8" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0.02</v>
+      </c>
       <c r="I8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J8" t="s">
         <v>111</v>
@@ -1753,20 +1775,20 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B10" t="s">
         <v>106</v>
       </c>
       <c r="C10" s="4">
         <f>C4*C6/C5</f>
-        <v>125.86727604735948</v>
+        <v>142.46515860305524</v>
       </c>
       <c r="D10" t="s">
         <v>115</v>
       </c>
       <c r="I10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J10" t="s">
         <v>138</v>
@@ -1823,7 +1845,7 @@
       </c>
       <c r="C2" s="4">
         <f>main!C10</f>
-        <v>125.86727604735948</v>
+        <v>142.46515860305524</v>
       </c>
     </row>
   </sheetData>
@@ -1911,11 +1933,78 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7967368-C341-4416-93F9-139A951A2B0D}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G31" xr:uid="{9E6C9298-4E19-408A-8A2C-0E94BEFA7393}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E31" xr:uid="{7C1A4F9C-04C2-49A1-92FA-70177C51AA50}">
+      <formula1>"Percentage,Absolute"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C31" xr:uid="{7C771BF8-FBC5-40DF-B642-0D5B9058415E}">
+      <formula1>"Activities,Commodities"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2BFD58C4-FDF4-4431-9E45-36B8D780538C}">
+          <x14:formula1>
+            <xm:f>indeces!$A$1:$A$111</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D31</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{768089DC-4ADE-4B4C-92C5-0B03079FFBA5}">
+          <x14:formula1>
+            <xm:f>indeces!$B$1:$B$23</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B31</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A31"/>
+    <sheetView zoomScale="295" zoomScaleNormal="295" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1961,26 +2050,26 @@
         <v>94</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G2" s="9">
         <f>-main!C8</f>
         <v>-0.26845637583892612</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1988,26 +2077,26 @@
         <v>95</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>41</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G3" s="10">
         <f>main!C7</f>
         <v>21.851454285957875</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>